<commit_message>
Minor edits to documentation in Powermax105 example template
</commit_message>
<xml_diff>
--- a/examples/powermax105_example_excel_template.xlsx
+++ b/examples/powermax105_example_excel_template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matthew.howe\Documents\cutchart-api-docs\examples\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia.johns\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC8F4CA-7F42-4EFE-91A0-B9A485D9F546}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F44935-FAB9-4531-99FA-E840F7C16835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cut" sheetId="1" r:id="rId1"/>
@@ -86,18 +86,9 @@
     <t>Base FeedRate</t>
   </si>
   <si>
-    <t>This column will automatically map to the MATERIAL data column because the name matches(case sensitive) and there is no explicit mapping provided.</t>
-  </si>
-  <si>
     <t>Unmapped data columns and unmapped custom columns will appear here and to the right.</t>
   </si>
   <si>
-    <t>This column's width will be adjusted by the width attribute in the xml transform.</t>
-  </si>
-  <si>
-    <t>This column is mapped to the BASE_FEEDRATE data column by the header attribute in the xml transform.</t>
-  </si>
-  <si>
     <t>PROFILE_TYPE</t>
   </si>
   <si>
@@ -105,18 +96,68 @@
   </si>
   <si>
     <t>PROFILE_AREA</t>
+  </si>
+  <si>
+    <t>This column will automatically map to the MATERIAL data column because the name matches (case sensitive) and there is no explicit mapping provided in the sample Powermax105 XML transform.</t>
+  </si>
+  <si>
+    <r>
+      <t>This column is mapped to the BASE_FEEDRATE data column by the header attribute in the</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> XML</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Tahoma"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color indexed="8"/>
+        <rFont val="Tahoma"/>
+        <family val="3"/>
+      </rPr>
+      <t>transform.</t>
+    </r>
+  </si>
+  <si>
+    <t>This column's width will be adjusted by the width attribute in the XML transform.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="8"/>
       <color indexed="8"/>
       <name val="Tahoma"/>
       <family val="3"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FFFF0000"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -139,9 +180,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -460,48 +504,46 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="32" customWidth="1" collapsed="1"/>
-    <col min="2" max="2" width="14.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="19.83203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="4" max="6" width="19.83203125" customWidth="1"/>
-    <col min="7" max="7" width="31.83203125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="19.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="9" max="9" width="13.5" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="10" max="10" width="50.5" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="14.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="19.85546875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="4" max="6" width="19.85546875" customWidth="1"/>
+    <col min="7" max="7" width="31.85546875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="19.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="9" max="9" width="13.42578125" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="10" max="10" width="50.42578125" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="28" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="12" max="12" width="27.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="13" max="13" width="21.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="29.33203125" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="23.5" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="12" max="12" width="27.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="13" max="13" width="21.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="29.28515625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="23.42578125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="16" max="16" width="20" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="17" max="17" width="17.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="18" max="18" width="16.6640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="19" max="19" width="20.1640625" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="20" max="20" width="18.5" customWidth="1" collapsed="1"/>
-    <col min="21" max="21" width="20.1640625" customWidth="1"/>
+    <col min="17" max="17" width="17.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="18" max="18" width="16.7109375" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="19" max="19" width="20.140625" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="20" max="20" width="18.42578125" customWidth="1" collapsed="1"/>
+    <col min="21" max="21" width="20.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" ht="57" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:21" ht="61.2" x14ac:dyDescent="0.2">
+      <c r="A1" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>19</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -512,13 +554,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="F2" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>
@@ -563,7 +605,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.15">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>16</v>
       </c>
@@ -584,6 +626,12 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101000CE7155E3050D34FAFA130CD16016A6B" ma:contentTypeVersion="10" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="9a21f13dcd64792f3f404864a5ea7ee8">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f6604700-c2bc-47ee-93e5-a018fac08543" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3d11fe5b1f126a37b5ee0bc1c38d816e" ns2:_="">
     <xsd:import namespace="f6604700-c2bc-47ee-93e5-a018fac08543"/>
@@ -767,12 +815,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5857B062-CFAE-4A91-B7AF-87697DAAFB8E}">
   <ds:schemaRefs>
@@ -782,6 +824,15 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9553E03-26FC-43F7-83E9-38234DCC426C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5C59672-5522-44B8-A0AA-330F0963C12D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -797,13 +848,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D9553E03-26FC-43F7-83E9-38234DCC426C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Powermax105 template, changed "data" to "database"
All columns are data columns, but not all columns are database columns.
</commit_message>
<xml_diff>
--- a/examples/powermax105_example_excel_template.xlsx
+++ b/examples/powermax105_example_excel_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\julia.johns\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69F44935-FAB9-4531-99FA-E840F7C16835}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46964CE0-4505-45D3-BE9F-D0D5EE335666}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -86,9 +86,6 @@
     <t>Base FeedRate</t>
   </si>
   <si>
-    <t>Unmapped data columns and unmapped custom columns will appear here and to the right.</t>
-  </si>
-  <si>
     <t>PROFILE_TYPE</t>
   </si>
   <si>
@@ -98,11 +95,14 @@
     <t>PROFILE_AREA</t>
   </si>
   <si>
-    <t>This column will automatically map to the MATERIAL data column because the name matches (case sensitive) and there is no explicit mapping provided in the sample Powermax105 XML transform.</t>
+    <t>This column's width will be adjusted by the width attribute in the XML transform.</t>
+  </si>
+  <si>
+    <t>This column will automatically map to the MATERIAL database column because the name matches (case sensitive) and there is no explicit mapping provided in the sample Powermax105 XML transform.</t>
   </si>
   <si>
     <r>
-      <t>This column is mapped to the BASE_FEEDRATE data column by the header attribute in the</t>
+      <t>This column is mapped to the BASE_FEEDRATE database column by the header attribute in the</t>
     </r>
     <r>
       <rPr>
@@ -133,7 +133,7 @@
     </r>
   </si>
   <si>
-    <t>This column's width will be adjusted by the width attribute in the XML transform.</t>
+    <t>Unmapped database columns and unmapped custom columns will appear here and to the right.</t>
   </si>
 </sst>
 </file>
@@ -504,7 +504,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:U3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="U30" sqref="U30"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
   <cols>
@@ -537,10 +539,10 @@
         <v>23</v>
       </c>
       <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>24</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.2">
@@ -554,13 +556,13 @@
         <v>4</v>
       </c>
       <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" t="s">
         <v>19</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>21</v>
       </c>
       <c r="G2" t="s">
         <v>17</v>

</xml_diff>